<commit_message>
Total Change in code of Master_Salary_TW removal of L&T code from whole site...
</commit_message>
<xml_diff>
--- a/media/COMBINED SALARY OF L_T AND IDFC TW/PER PAID CASE(Including Fixed Salary) IDFC-TW.xlsx
+++ b/media/COMBINED SALARY OF L_T AND IDFC TW/PER PAID CASE(Including Fixed Salary) IDFC-TW.xlsx
@@ -3085,7 +3085,9 @@
       <c r="AC20" t="n">
         <v>300</v>
       </c>
-      <c r="AD20" t="inlineStr"/>
+      <c r="AD20" t="n">
+        <v>0</v>
+      </c>
       <c r="AE20" t="inlineStr"/>
       <c r="AF20" t="inlineStr">
         <is>
@@ -3611,7 +3613,9 @@
       <c r="AC24" t="n">
         <v>200</v>
       </c>
-      <c r="AD24" t="inlineStr"/>
+      <c r="AD24" t="n">
+        <v>0</v>
+      </c>
       <c r="AE24" t="inlineStr"/>
       <c r="AF24" t="inlineStr">
         <is>
@@ -4136,7 +4140,7 @@
         <v>2500</v>
       </c>
       <c r="AD28" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" t="inlineStr">

</xml_diff>